<commit_message>
add hasil apriori dan asosiasi tahun 2020
</commit_message>
<xml_diff>
--- a/data/hasil_apriori_up_3.xlsx
+++ b/data/hasil_apriori_up_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,31 +447,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.1687841891653432</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>frozenset({'Oli Gardan'})</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>frozenset({'Oli Mesin Matic'})</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>frozenset({'Oli Mesin Matic', 'Oli Gardan'})</t>
+          <t>frozenset({'Mpx 2 10W 30 Sl 800 mL'})</t>
         </is>
       </c>
     </row>

</xml_diff>